<commit_message>
Ajustes escaleta y mapa conceptual guion CN_06_02_CO
Ajustes escaleta y mapa conceptual guion CN_06_02_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/Escaleta CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/Escaleta CN_06_02_CO.xlsx
@@ -2121,8 +2121,29 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2130,33 +2151,12 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2169,6 +2169,57 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2189,57 +2240,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4507,9 +4507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4542,50 +4542,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="142" t="s">
+      <c r="C1" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="131" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="135" t="s">
+      <c r="E1" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="132" t="s">
+      <c r="F1" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="137" t="s">
+      <c r="G1" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="132" t="s">
+      <c r="H1" s="139" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="132" t="s">
+      <c r="I1" s="139" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="139" t="s">
+      <c r="J1" s="134" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="138" t="s">
+      <c r="K1" s="133" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="137" t="s">
+      <c r="L1" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="140" t="s">
+      <c r="M1" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="141"/>
-      <c r="O1" s="134" t="s">
+      <c r="N1" s="136"/>
+      <c r="O1" s="142" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="134" t="s">
+      <c r="P1" s="142" t="s">
         <v>116</v>
       </c>
       <c r="Q1" s="144" t="s">
@@ -4603,32 +4603,32 @@
       <c r="U1" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="X1" s="131" t="s">
+      <c r="X1" s="141" t="s">
         <v>309</v>
       </c>
-      <c r="Y1" s="131"/>
-      <c r="Z1" s="131"/>
+      <c r="Y1" s="141"/>
+      <c r="Z1" s="141"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136"/>
-      <c r="B2" s="135"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="137"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="137"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="133"/>
+      <c r="L2" s="132"/>
       <c r="M2" s="15" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="134"/>
+      <c r="O2" s="142"/>
       <c r="P2" s="143"/>
       <c r="Q2" s="144"/>
       <c r="R2" s="146"/>
@@ -6826,7 +6826,9 @@
       <c r="G37" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="H37" s="22"/>
+      <c r="H37" s="22">
+        <v>33</v>
+      </c>
       <c r="I37" s="16"/>
       <c r="J37" s="26"/>
       <c r="K37" s="11"/>
@@ -6866,7 +6868,7 @@
         <v>221</v>
       </c>
       <c r="H38" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>134</v>
@@ -6919,7 +6921,7 @@
         <v>228</v>
       </c>
       <c r="H39" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I39" s="16" t="s">
         <v>134</v>
@@ -7189,16 +7191,6 @@
   </sheetData>
   <autoFilter ref="A2:U39"/>
   <mergeCells count="21">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="X1:Z1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -7210,6 +7202,16 @@
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P41 I3:I41">
@@ -7582,30 +7584,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="147" t="s">
+      <c r="B2" s="164" t="s">
         <v>270</v>
       </c>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="148"/>
-      <c r="H2" s="149"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="166"/>
     </row>
     <row r="3" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="46"/>
-      <c r="C3" s="150" t="s">
+      <c r="C3" s="167" t="s">
         <v>271</v>
       </c>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150" t="s">
+      <c r="D3" s="167"/>
+      <c r="E3" s="167" t="s">
         <v>272</v>
       </c>
-      <c r="F3" s="151"/>
-      <c r="G3" s="152" t="s">
+      <c r="F3" s="168"/>
+      <c r="G3" s="169" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="153"/>
+      <c r="H3" s="170"/>
     </row>
     <row r="4" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47"/>
@@ -7759,37 +7761,37 @@
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="157" t="s">
+      <c r="B12" s="150" t="s">
         <v>277</v>
       </c>
-      <c r="C12" s="158"/>
-      <c r="D12" s="158"/>
-      <c r="E12" s="158"/>
-      <c r="F12" s="158"/>
-      <c r="G12" s="158"/>
-      <c r="H12" s="158"/>
-      <c r="I12" s="159"/>
+      <c r="C12" s="151"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="152"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="153" t="s">
         <v>278</v>
       </c>
-      <c r="C13" s="162" t="s">
+      <c r="C13" s="155" t="s">
         <v>271</v>
       </c>
-      <c r="D13" s="163"/>
-      <c r="E13" s="164" t="s">
+      <c r="D13" s="156"/>
+      <c r="E13" s="157" t="s">
         <v>272</v>
       </c>
-      <c r="F13" s="165"/>
-      <c r="G13" s="166" t="s">
+      <c r="F13" s="158"/>
+      <c r="G13" s="159" t="s">
         <v>273</v>
       </c>
-      <c r="H13" s="167"/>
-      <c r="I13" s="168"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="161"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="161"/>
+      <c r="B14" s="154"/>
       <c r="C14" s="69" t="s">
         <v>274</v>
       </c>
@@ -7955,13 +7957,13 @@
       <c r="I20" s="111"/>
     </row>
     <row r="21" spans="1:9" ht="31.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="169" t="s">
+      <c r="B21" s="162" t="s">
         <v>280</v>
       </c>
-      <c r="C21" s="170"/>
+      <c r="C21" s="163"/>
     </row>
     <row r="22" spans="1:9" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="154" t="s">
+      <c r="B22" s="147" t="s">
         <v>281</v>
       </c>
       <c r="C22" s="112" t="s">
@@ -7972,7 +7974,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="155"/>
+      <c r="B23" s="148"/>
       <c r="C23" s="113" t="s">
         <v>284</v>
       </c>
@@ -7981,7 +7983,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="155"/>
+      <c r="B24" s="148"/>
       <c r="C24" s="113" t="s">
         <v>70</v>
       </c>
@@ -8001,7 +8003,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="154" t="s">
+      <c r="B26" s="147" t="s">
         <v>287</v>
       </c>
       <c r="C26" s="112" t="s">
@@ -8009,19 +8011,19 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="155"/>
+      <c r="B27" s="148"/>
       <c r="C27" s="113" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="155"/>
+      <c r="B28" s="148"/>
       <c r="C28" s="116" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="156"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="117" t="s">
         <v>74</v>
       </c>
@@ -8036,6 +8038,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B22:B24"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B13:B14"/>
@@ -8043,11 +8050,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización archivos guion CN_06_02_CO
Incluye reorganización de archivos, actualización escaleta y solicitudes
gráficas de recursos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/Escaleta CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/Escaleta CN_06_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,8 +23,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>diego m.</author>
+  </authors>
+  <commentList>
+    <comment ref="G15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>diego m.:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Anterior nombre "La estructura de la célula",   en escaleta Oliver "La estructura de la célula - nuevo"
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="270">
   <si>
     <t>Asignatura</t>
   </si>
@@ -525,9 +560,6 @@
     <t>Consolidación</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La célula, su estructura y su función</t>
-  </si>
-  <si>
     <t>Actividad sobre la célula y su función</t>
   </si>
   <si>
@@ -597,9 +629,6 @@
     <t>Los tejidos del cuerpo humano</t>
   </si>
   <si>
-    <t>Actividad que permite identificar la clasificación de los tejidos del cuerpo humano</t>
-  </si>
-  <si>
     <t>Recurso M4A-01</t>
   </si>
   <si>
@@ -829,13 +858,25 @@
   </si>
   <si>
     <t>Link del recurso en Aula Planeta es: http://editorial.profesores.aulaplaneta.com//DesktopModules/PPP_UploadScorms/RecursoPopUp.aspx?RecursoID=524976                                            En la segunda pantalla, cambiar la palabra “Completar” por la palabra “Completa”</t>
+  </si>
+  <si>
+    <t>Reconce los diferentes tipos de células</t>
+  </si>
+  <si>
+    <t>La célula,  estructura y su función</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La célula, estructura y su función</t>
+  </si>
+  <si>
+    <t>Actividad que permite identificar los tejidos del cuerpo humano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -903,6 +944,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1057,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1131,9 +1185,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1227,6 +1278,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1532,12 +1589,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,94 +1622,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" s="41" t="s">
+      <c r="N1" s="60"/>
+      <c r="O1" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="S1" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="T1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="54"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="38" t="s">
+      <c r="A2" s="53"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="44"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1665,11 +1722,11 @@
         <v>124</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>125</v>
+        <v>267</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="64" t="s">
         <v>126</v>
       </c>
       <c r="H3" s="31">
@@ -1678,7 +1735,7 @@
       <c r="I3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="63" t="s">
         <v>128</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -1691,7 +1748,7 @@
         <v>117</v>
       </c>
       <c r="N3" s="8"/>
-      <c r="O3" s="34"/>
+      <c r="O3" s="33"/>
       <c r="P3" s="9" t="s">
         <v>19</v>
       </c>
@@ -1704,7 +1761,7 @@
       <c r="S3" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="T3" s="36" t="s">
         <v>131</v>
       </c>
       <c r="U3" s="10" t="s">
@@ -1721,17 +1778,17 @@
       <c r="C4" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>125</v>
+      <c r="D4" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>133</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="32">
         <v>2</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -1747,10 +1804,10 @@
         <v>8</v>
       </c>
       <c r="M4" s="8"/>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="33" t="s">
         <v>137</v>
       </c>
       <c r="P4" s="9" t="s">
@@ -1765,7 +1822,7 @@
       <c r="S4" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T4" s="37" t="s">
+      <c r="T4" s="36" t="s">
         <v>134</v>
       </c>
       <c r="U4" s="10" t="s">
@@ -1782,23 +1839,23 @@
       <c r="C5" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>125</v>
+      <c r="D5" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>133</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="32">
         <v>3</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="16" t="s">
         <v>142</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1811,7 +1868,7 @@
       <c r="N5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="34"/>
+      <c r="O5" s="33"/>
       <c r="P5" s="9" t="s">
         <v>19</v>
       </c>
@@ -1824,7 +1881,7 @@
       <c r="S5" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T5" s="34" t="s">
+      <c r="T5" s="36" t="s">
         <v>144</v>
       </c>
       <c r="U5" s="10" t="s">
@@ -1838,30 +1895,30 @@
       <c r="B6" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>125</v>
+      <c r="D6" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>146</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="5"/>
       <c r="J6" s="16"/>
       <c r="K6" s="7"/>
       <c r="L6" s="6"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="34"/>
+      <c r="O6" s="33"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="11"/>
       <c r="S6" s="10"/>
-      <c r="T6" s="37"/>
+      <c r="T6" s="36"/>
       <c r="U6" s="10"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1874,23 +1931,23 @@
       <c r="C7" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>125</v>
+      <c r="D7" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>147</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="32">
         <v>4</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="16" t="s">
         <v>149</v>
       </c>
       <c r="K7" s="7" t="s">
@@ -1903,7 +1960,7 @@
         <v>54</v>
       </c>
       <c r="N7" s="8"/>
-      <c r="O7" s="34"/>
+      <c r="O7" s="33"/>
       <c r="P7" s="9" t="s">
         <v>19</v>
       </c>
@@ -1916,7 +1973,7 @@
       <c r="S7" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="T7" s="34" t="s">
+      <c r="T7" s="36" t="s">
         <v>152</v>
       </c>
       <c r="U7" s="10" t="s">
@@ -1933,17 +1990,17 @@
       <c r="C8" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>125</v>
+      <c r="D8" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>147</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="32">
         <v>5</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -1959,10 +2016,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="8"/>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="34" t="s">
+      <c r="O8" s="33" t="s">
         <v>156</v>
       </c>
       <c r="P8" s="9" t="s">
@@ -1977,7 +2034,7 @@
       <c r="S8" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="T8" s="37" t="s">
+      <c r="T8" s="36" t="s">
         <v>154</v>
       </c>
       <c r="U8" s="10" t="s">
@@ -1994,23 +2051,23 @@
       <c r="C9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>125</v>
+      <c r="D9" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>147</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="32">
         <v>6</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="16" t="s">
         <v>162</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -2023,7 +2080,7 @@
       <c r="N9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="34"/>
+      <c r="O9" s="33"/>
       <c r="P9" s="9" t="s">
         <v>20</v>
       </c>
@@ -2036,7 +2093,7 @@
       <c r="S9" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="T9" s="36" t="s">
         <v>163</v>
       </c>
       <c r="U9" s="10" t="s">
@@ -2053,24 +2110,24 @@
       <c r="C10" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>125</v>
+      <c r="D10" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>147</v>
       </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="32">
         <v>7</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>127</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>19</v>
@@ -2078,12 +2135,12 @@
       <c r="L10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="39"/>
-      <c r="O10" s="34" t="s">
-        <v>267</v>
+      <c r="N10" s="38"/>
+      <c r="O10" s="33" t="s">
+        <v>265</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -2091,7 +2148,7 @@
       <c r="Q10" s="10"/>
       <c r="R10" s="11"/>
       <c r="S10" s="10"/>
-      <c r="T10" s="37"/>
+      <c r="T10" s="36"/>
       <c r="U10" s="10"/>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2104,24 +2161,24 @@
       <c r="C11" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>125</v>
+      <c r="D11" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>165</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="H11" s="33">
+      <c r="G11" s="35" t="s">
+        <v>268</v>
+      </c>
+      <c r="H11" s="32">
         <v>8</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2130,10 +2187,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="39" t="s">
+      <c r="N11" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="O11" s="34"/>
+      <c r="O11" s="33"/>
       <c r="P11" s="9" t="s">
         <v>19</v>
       </c>
@@ -2146,8 +2203,8 @@
       <c r="S11" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T11" s="37" t="s">
-        <v>168</v>
+      <c r="T11" s="36" t="s">
+        <v>167</v>
       </c>
       <c r="U11" s="10" t="s">
         <v>140</v>
@@ -2164,26 +2221,26 @@
         <v>124</v>
       </c>
       <c r="D12" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>170</v>
-      </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="33"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="5"/>
       <c r="J12" s="16"/>
       <c r="K12" s="7"/>
       <c r="L12" s="6"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="34"/>
+      <c r="O12" s="33"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
       <c r="S12" s="10"/>
-      <c r="T12" s="37"/>
+      <c r="T12" s="36"/>
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2197,23 +2254,23 @@
         <v>124</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="32">
         <v>9</v>
       </c>
       <c r="I13" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="J13" s="34" t="s">
-        <v>172</v>
+      <c r="J13" s="16" t="s">
+        <v>171</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>20</v>
@@ -2225,7 +2282,7 @@
         <v>57</v>
       </c>
       <c r="N13" s="8"/>
-      <c r="O13" s="34"/>
+      <c r="O13" s="33"/>
       <c r="P13" s="9" t="s">
         <v>19</v>
       </c>
@@ -2238,8 +2295,8 @@
       <c r="S13" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="T13" s="34" t="s">
-        <v>173</v>
+      <c r="T13" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="U13" s="10" t="s">
         <v>153</v>
@@ -2256,23 +2313,23 @@
         <v>124</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="33">
+      <c r="G14" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" s="32">
         <v>10</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>127</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>20</v>
@@ -2284,7 +2341,7 @@
         <v>117</v>
       </c>
       <c r="N14" s="8"/>
-      <c r="O14" s="34"/>
+      <c r="O14" s="33"/>
       <c r="P14" s="9" t="s">
         <v>19</v>
       </c>
@@ -2297,8 +2354,8 @@
       <c r="S14" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="T14" s="37" t="s">
-        <v>176</v>
+      <c r="T14" s="36" t="s">
+        <v>175</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>132</v>
@@ -2315,23 +2372,23 @@
         <v>124</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15" s="9"/>
-      <c r="G15" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="H15" s="33">
+      <c r="G15" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="H15" s="32">
         <v>11</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>127</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>19</v>
@@ -2339,12 +2396,12 @@
       <c r="L15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="39" t="s">
+      <c r="M15" s="38" t="s">
         <v>57</v>
       </c>
       <c r="N15" s="8"/>
-      <c r="O15" s="34" t="s">
-        <v>178</v>
+      <c r="O15" s="33" t="s">
+        <v>177</v>
       </c>
       <c r="P15" s="9" t="s">
         <v>19</v>
@@ -2358,7 +2415,7 @@
       <c r="S15" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="T15" s="37" t="s">
+      <c r="T15" s="36" t="s">
         <v>164</v>
       </c>
       <c r="U15" s="10" t="s">
@@ -2376,23 +2433,23 @@
         <v>124</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F16" s="9"/>
-      <c r="G16" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="H16" s="33">
+      <c r="G16" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="32">
         <v>12</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="34" t="s">
-        <v>180</v>
+      <c r="J16" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2404,7 +2461,7 @@
       <c r="N16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="O16" s="34"/>
+      <c r="O16" s="33"/>
       <c r="P16" s="9" t="s">
         <v>20</v>
       </c>
@@ -2417,8 +2474,8 @@
       <c r="S16" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T16" s="34" t="s">
-        <v>181</v>
+      <c r="T16" s="36" t="s">
+        <v>180</v>
       </c>
       <c r="U16" s="10" t="s">
         <v>145</v>
@@ -2435,23 +2492,23 @@
         <v>124</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>165</v>
       </c>
       <c r="F17" s="9"/>
-      <c r="G17" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" s="33">
+      <c r="G17" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="H17" s="32">
         <v>13</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="34" t="s">
-        <v>183</v>
+      <c r="J17" s="16" t="s">
+        <v>182</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2460,10 +2517,10 @@
         <v>8</v>
       </c>
       <c r="M17" s="8"/>
-      <c r="N17" s="40" t="s">
+      <c r="N17" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="34"/>
+      <c r="O17" s="33"/>
       <c r="P17" s="9" t="s">
         <v>19</v>
       </c>
@@ -2476,8 +2533,8 @@
       <c r="S17" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T17" s="34" t="s">
-        <v>184</v>
+      <c r="T17" s="36" t="s">
+        <v>183</v>
       </c>
       <c r="U17" s="10" t="s">
         <v>145</v>
@@ -2494,21 +2551,21 @@
         <v>124</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="H18" s="33">
+      <c r="G18" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" s="32">
         <v>14</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J18" s="34" t="s">
-        <v>187</v>
+      <c r="J18" s="16" t="s">
+        <v>186</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2520,7 +2577,7 @@
       <c r="N18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="34"/>
+      <c r="O18" s="33"/>
       <c r="P18" s="9" t="s">
         <v>19</v>
       </c>
@@ -2533,14 +2590,14 @@
       <c r="S18" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T18" s="34" t="s">
-        <v>188</v>
+      <c r="T18" s="36" t="s">
+        <v>187</v>
       </c>
       <c r="U18" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
@@ -2551,33 +2608,37 @@
         <v>124</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="E19" s="15"/>
+        <v>184</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>190</v>
+      </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="H19" s="33">
+      <c r="G19" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="H19" s="32">
         <v>15</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>190</v>
+        <v>127</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>192</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O19" s="34"/>
+        <v>5</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="N19" s="8"/>
+      <c r="O19" s="33" t="s">
+        <v>193</v>
+      </c>
       <c r="P19" s="9" t="s">
         <v>19</v>
       </c>
@@ -2585,19 +2646,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="T19" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="T19" s="36" t="s">
         <v>191</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>122</v>
       </c>
@@ -2608,23 +2669,23 @@
         <v>124</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F20" s="9"/>
-      <c r="G20" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="H20" s="33">
+      <c r="G20" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="32">
         <v>16</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>19</v>
@@ -2632,12 +2693,12 @@
       <c r="L20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="34" t="s">
-        <v>195</v>
+      <c r="M20" s="8"/>
+      <c r="N20" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="33" t="s">
+        <v>137</v>
       </c>
       <c r="P20" s="9" t="s">
         <v>19</v>
@@ -2651,8 +2712,8 @@
       <c r="S20" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T20" s="37" t="s">
-        <v>193</v>
+      <c r="T20" s="36" t="s">
+        <v>194</v>
       </c>
       <c r="U20" s="10" t="s">
         <v>140</v>
@@ -2669,37 +2730,33 @@
         <v>124</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>192</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E21" s="15"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="H21" s="33">
+      <c r="G21" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" s="32">
         <v>17</v>
       </c>
       <c r="I21" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>197</v>
+        <v>269</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M21" s="8"/>
-      <c r="N21" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="O21" s="34" t="s">
-        <v>137</v>
-      </c>
+      <c r="N21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" s="33"/>
       <c r="P21" s="9" t="s">
         <v>19</v>
       </c>
@@ -2707,16 +2764,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="T21" s="37" t="s">
-        <v>196</v>
+        <v>143</v>
+      </c>
+      <c r="T21" s="36" t="s">
+        <v>189</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2730,23 +2787,23 @@
         <v>124</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="H22" s="33">
+      <c r="G22" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="H22" s="32">
         <v>18</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>19</v>
@@ -2755,10 +2812,10 @@
         <v>5</v>
       </c>
       <c r="M22" s="8"/>
-      <c r="N22" s="39" t="s">
+      <c r="N22" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="34" t="s">
+      <c r="O22" s="33" t="s">
         <v>137</v>
       </c>
       <c r="P22" s="9" t="s">
@@ -2773,8 +2830,8 @@
       <c r="S22" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T22" s="37" t="s">
-        <v>199</v>
+      <c r="T22" s="36" t="s">
+        <v>197</v>
       </c>
       <c r="U22" s="10" t="s">
         <v>140</v>
@@ -2791,23 +2848,23 @@
         <v>124</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>165</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="G23" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="H23" s="33">
+      <c r="G23" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="H23" s="32">
         <v>19</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>19</v>
@@ -2816,11 +2873,11 @@
         <v>8</v>
       </c>
       <c r="M23" s="8"/>
-      <c r="N23" s="39" t="s">
+      <c r="N23" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="O23" s="34" t="s">
-        <v>203</v>
+      <c r="O23" s="33" t="s">
+        <v>201</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>19</v>
@@ -2834,8 +2891,8 @@
       <c r="S23" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T23" s="37" t="s">
-        <v>204</v>
+      <c r="T23" s="36" t="s">
+        <v>202</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>140</v>
@@ -2852,21 +2909,21 @@
         <v>124</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="36" t="s">
-        <v>206</v>
-      </c>
-      <c r="H24" s="33">
+      <c r="G24" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24" s="32">
         <v>20</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>127</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>19</v>
@@ -2874,12 +2931,12 @@
       <c r="L24" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M24" s="39" t="s">
+      <c r="M24" s="38" t="s">
         <v>117</v>
       </c>
       <c r="N24" s="8"/>
-      <c r="O24" s="34" t="s">
-        <v>208</v>
+      <c r="O24" s="33" t="s">
+        <v>206</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>19</v>
@@ -2893,8 +2950,8 @@
       <c r="S24" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T24" s="37" t="s">
-        <v>206</v>
+      <c r="T24" s="36" t="s">
+        <v>204</v>
       </c>
       <c r="U24" s="10" t="s">
         <v>140</v>
@@ -2911,23 +2968,23 @@
         <v>124</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F25" s="9"/>
-      <c r="G25" s="36" t="s">
-        <v>210</v>
-      </c>
-      <c r="H25" s="33">
+      <c r="G25" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="H25" s="32">
         <v>21</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>19</v>
@@ -2936,11 +2993,11 @@
         <v>5</v>
       </c>
       <c r="M25" s="8"/>
-      <c r="N25" s="39" t="s">
+      <c r="N25" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="O25" s="34" t="s">
-        <v>208</v>
+      <c r="O25" s="33" t="s">
+        <v>206</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>19</v>
@@ -2954,8 +3011,8 @@
       <c r="S25" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T25" s="37" t="s">
-        <v>210</v>
+      <c r="T25" s="36" t="s">
+        <v>208</v>
       </c>
       <c r="U25" s="10" t="s">
         <v>140</v>
@@ -2972,23 +3029,23 @@
         <v>124</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>165</v>
       </c>
       <c r="F26" s="9"/>
-      <c r="G26" s="36" t="s">
-        <v>212</v>
-      </c>
-      <c r="H26" s="33">
+      <c r="G26" s="35" t="s">
+        <v>210</v>
+      </c>
+      <c r="H26" s="32">
         <v>22</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>19</v>
@@ -2997,11 +3054,11 @@
         <v>8</v>
       </c>
       <c r="M26" s="8"/>
-      <c r="N26" s="39" t="s">
+      <c r="N26" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="34" t="s">
-        <v>214</v>
+      <c r="O26" s="33" t="s">
+        <v>212</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>19</v>
@@ -3015,8 +3072,8 @@
       <c r="S26" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T26" s="37" t="s">
-        <v>212</v>
+      <c r="T26" s="36" t="s">
+        <v>210</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>140</v>
@@ -3033,23 +3090,23 @@
         <v>124</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>165</v>
       </c>
       <c r="F27" s="9"/>
-      <c r="G27" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="H27" s="33">
+      <c r="G27" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="H27" s="32">
         <v>23</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J27" s="34" t="s">
-        <v>216</v>
+      <c r="J27" s="16" t="s">
+        <v>214</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -3058,10 +3115,10 @@
         <v>8</v>
       </c>
       <c r="M27" s="8"/>
-      <c r="N27" s="40" t="s">
+      <c r="N27" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="O27" s="34"/>
+      <c r="O27" s="33"/>
       <c r="P27" s="9" t="s">
         <v>19</v>
       </c>
@@ -3074,8 +3131,8 @@
       <c r="S27" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T27" s="34" t="s">
-        <v>217</v>
+      <c r="T27" s="36" t="s">
+        <v>215</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>145</v>
@@ -3092,21 +3149,21 @@
         <v>124</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="H28" s="33">
+      <c r="G28" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H28" s="32">
         <v>24</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>19</v>
@@ -3115,10 +3172,10 @@
         <v>8</v>
       </c>
       <c r="M28" s="8"/>
-      <c r="N28" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="O28" s="34"/>
+      <c r="N28" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="O28" s="33"/>
       <c r="P28" s="9" t="s">
         <v>19</v>
       </c>
@@ -3131,8 +3188,8 @@
       <c r="S28" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T28" s="37" t="s">
-        <v>219</v>
+      <c r="T28" s="36" t="s">
+        <v>217</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>140</v>
@@ -3149,21 +3206,21 @@
         <v>124</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="H29" s="33">
+      <c r="G29" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="H29" s="32">
         <v>25</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>19</v>
@@ -3172,10 +3229,10 @@
         <v>8</v>
       </c>
       <c r="M29" s="8"/>
-      <c r="N29" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="O29" s="34"/>
+      <c r="N29" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="O29" s="33"/>
       <c r="P29" s="9" t="s">
         <v>19</v>
       </c>
@@ -3188,8 +3245,8 @@
       <c r="S29" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T29" s="37" t="s">
-        <v>222</v>
+      <c r="T29" s="36" t="s">
+        <v>220</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>140</v>
@@ -3206,21 +3263,21 @@
         <v>124</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="H30" s="33">
+      <c r="G30" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="H30" s="32">
         <v>26</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>19</v>
@@ -3229,11 +3286,11 @@
         <v>8</v>
       </c>
       <c r="M30" s="8"/>
-      <c r="N30" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="O30" s="34" t="s">
-        <v>226</v>
+      <c r="N30" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="O30" s="33" t="s">
+        <v>224</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>19</v>
@@ -3247,8 +3304,8 @@
       <c r="S30" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T30" s="37" t="s">
-        <v>224</v>
+      <c r="T30" s="36" t="s">
+        <v>222</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>140</v>
@@ -3265,21 +3322,21 @@
         <v>124</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E31" s="15"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="H31" s="33">
+      <c r="G31" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="H31" s="32">
         <v>27</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>19</v>
@@ -3288,11 +3345,11 @@
         <v>8</v>
       </c>
       <c r="M31" s="8"/>
-      <c r="N31" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="O31" s="34" t="s">
-        <v>229</v>
+      <c r="N31" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="O31" s="33" t="s">
+        <v>227</v>
       </c>
       <c r="P31" s="9" t="s">
         <v>19</v>
@@ -3306,8 +3363,8 @@
       <c r="S31" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T31" s="37" t="s">
-        <v>227</v>
+      <c r="T31" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>140</v>
@@ -3324,21 +3381,21 @@
         <v>124</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="H32" s="33">
+      <c r="G32" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="H32" s="32">
         <v>28</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>19</v>
@@ -3347,11 +3404,11 @@
         <v>8</v>
       </c>
       <c r="M32" s="8"/>
-      <c r="N32" s="39" t="s">
-        <v>221</v>
-      </c>
-      <c r="O32" s="34" t="s">
-        <v>232</v>
+      <c r="N32" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="O32" s="33" t="s">
+        <v>230</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>19</v>
@@ -3365,8 +3422,8 @@
       <c r="S32" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="T32" s="37" t="s">
-        <v>230</v>
+      <c r="T32" s="36" t="s">
+        <v>228</v>
       </c>
       <c r="U32" s="10" t="s">
         <v>140</v>
@@ -3383,19 +3440,19 @@
         <v>124</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="36" t="s">
+      <c r="G33" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="33">
+      <c r="H33" s="32">
         <v>29</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K33" s="7"/>
       <c r="L33" s="6" t="s">
@@ -3403,14 +3460,14 @@
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
-      <c r="O33" s="34"/>
+      <c r="O33" s="33"/>
       <c r="P33" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="10"/>
       <c r="R33" s="11"/>
       <c r="S33" s="10"/>
-      <c r="T33" s="37"/>
+      <c r="T33" s="36"/>
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3424,21 +3481,21 @@
         <v>124</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="H34" s="33">
+      <c r="G34" s="35" t="s">
+        <v>233</v>
+      </c>
+      <c r="H34" s="32">
         <v>30</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>135</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3450,7 +3507,7 @@
       <c r="N34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="34"/>
+      <c r="O34" s="33"/>
       <c r="P34" s="9" t="s">
         <v>19</v>
       </c>
@@ -3463,8 +3520,8 @@
       <c r="S34" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T34" s="37" t="s">
-        <v>237</v>
+      <c r="T34" s="36" t="s">
+        <v>235</v>
       </c>
       <c r="U34" s="10" t="s">
         <v>145</v>
@@ -3483,17 +3540,17 @@
       <c r="D35" s="14"/>
       <c r="E35" s="15"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="H35" s="33">
+      <c r="G35" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="H35" s="32">
         <v>31</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="J35" s="34" t="s">
-        <v>265</v>
+      <c r="J35" s="16" t="s">
+        <v>263</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3505,7 +3562,7 @@
       <c r="N35" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="O35" s="34"/>
+      <c r="O35" s="33"/>
       <c r="P35" s="9" t="s">
         <v>20</v>
       </c>
@@ -3518,8 +3575,8 @@
       <c r="S35" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="T35" s="34" t="s">
-        <v>239</v>
+      <c r="T35" s="36" t="s">
+        <v>237</v>
       </c>
       <c r="U35" s="10" t="s">
         <v>145</v>
@@ -3532,7 +3589,7 @@
       <c r="D36" s="14"/>
       <c r="E36" s="15"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="36"/>
+      <c r="G36" s="35"/>
       <c r="H36" s="9"/>
       <c r="I36" s="5"/>
       <c r="J36" s="16"/>
@@ -3545,7 +3602,7 @@
       <c r="Q36" s="10"/>
       <c r="R36" s="11"/>
       <c r="S36" s="10"/>
-      <c r="T36" s="37"/>
+      <c r="T36" s="36"/>
       <c r="U36" s="10"/>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3555,7 +3612,7 @@
       <c r="D37" s="14"/>
       <c r="E37" s="15"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="36"/>
+      <c r="G37" s="35"/>
       <c r="H37" s="9"/>
       <c r="I37" s="5"/>
       <c r="J37" s="16"/>
@@ -3568,7 +3625,7 @@
       <c r="Q37" s="10"/>
       <c r="R37" s="11"/>
       <c r="S37" s="10"/>
-      <c r="T37" s="37"/>
+      <c r="T37" s="36"/>
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3578,7 +3635,7 @@
       <c r="D38" s="14"/>
       <c r="E38" s="15"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="36"/>
+      <c r="G38" s="35"/>
       <c r="H38" s="9"/>
       <c r="I38" s="5"/>
       <c r="J38" s="16"/>
@@ -3591,7 +3648,7 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="11"/>
       <c r="S38" s="10"/>
-      <c r="T38" s="37"/>
+      <c r="T38" s="36"/>
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3601,7 +3658,7 @@
       <c r="D39" s="14"/>
       <c r="E39" s="15"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="36"/>
+      <c r="G39" s="35"/>
       <c r="H39" s="9"/>
       <c r="I39" s="5"/>
       <c r="J39" s="16"/>
@@ -3614,7 +3671,7 @@
       <c r="Q39" s="10"/>
       <c r="R39" s="11"/>
       <c r="S39" s="10"/>
-      <c r="T39" s="37"/>
+      <c r="T39" s="36"/>
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3624,7 +3681,7 @@
       <c r="D40" s="14"/>
       <c r="E40" s="15"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="36"/>
+      <c r="G40" s="35"/>
       <c r="H40" s="9"/>
       <c r="I40" s="5"/>
       <c r="J40" s="16"/>
@@ -3637,7 +3694,7 @@
       <c r="Q40" s="10"/>
       <c r="R40" s="11"/>
       <c r="S40" s="10"/>
-      <c r="T40" s="37"/>
+      <c r="T40" s="36"/>
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3647,7 +3704,7 @@
       <c r="D41" s="14"/>
       <c r="E41" s="15"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="36"/>
+      <c r="G41" s="35"/>
       <c r="H41" s="9"/>
       <c r="I41" s="5"/>
       <c r="J41" s="16"/>
@@ -3660,7 +3717,7 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="11"/>
       <c r="S41" s="10"/>
-      <c r="T41" s="37"/>
+      <c r="T41" s="36"/>
       <c r="U41" s="10"/>
     </row>
     <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3670,7 +3727,7 @@
       <c r="D42" s="14"/>
       <c r="E42" s="15"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="36"/>
+      <c r="G42" s="35"/>
       <c r="H42" s="9"/>
       <c r="I42" s="5"/>
       <c r="J42" s="16"/>
@@ -3683,7 +3740,7 @@
       <c r="Q42" s="10"/>
       <c r="R42" s="11"/>
       <c r="S42" s="10"/>
-      <c r="T42" s="37"/>
+      <c r="T42" s="36"/>
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3693,7 +3750,7 @@
       <c r="D43" s="14"/>
       <c r="E43" s="15"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="36"/>
+      <c r="G43" s="35"/>
       <c r="H43" s="9"/>
       <c r="I43" s="5"/>
       <c r="J43" s="16"/>
@@ -3706,7 +3763,7 @@
       <c r="Q43" s="10"/>
       <c r="R43" s="11"/>
       <c r="S43" s="10"/>
-      <c r="T43" s="37"/>
+      <c r="T43" s="36"/>
       <c r="U43" s="10"/>
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3716,7 +3773,7 @@
       <c r="D44" s="14"/>
       <c r="E44" s="15"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="36"/>
+      <c r="G44" s="35"/>
       <c r="H44" s="9"/>
       <c r="I44" s="5"/>
       <c r="J44" s="16"/>
@@ -3729,7 +3786,7 @@
       <c r="Q44" s="10"/>
       <c r="R44" s="11"/>
       <c r="S44" s="10"/>
-      <c r="T44" s="37"/>
+      <c r="T44" s="36"/>
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3739,7 +3796,7 @@
       <c r="D45" s="14"/>
       <c r="E45" s="15"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="36"/>
+      <c r="G45" s="35"/>
       <c r="H45" s="9"/>
       <c r="I45" s="5"/>
       <c r="J45" s="16"/>
@@ -3752,7 +3809,7 @@
       <c r="Q45" s="10"/>
       <c r="R45" s="11"/>
       <c r="S45" s="10"/>
-      <c r="T45" s="37"/>
+      <c r="T45" s="36"/>
       <c r="U45" s="10"/>
     </row>
     <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3762,7 +3819,7 @@
       <c r="D46" s="14"/>
       <c r="E46" s="15"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="36"/>
+      <c r="G46" s="35"/>
       <c r="H46" s="9"/>
       <c r="I46" s="5"/>
       <c r="J46" s="16"/>
@@ -3775,7 +3832,7 @@
       <c r="Q46" s="10"/>
       <c r="R46" s="11"/>
       <c r="S46" s="10"/>
-      <c r="T46" s="37"/>
+      <c r="T46" s="36"/>
       <c r="U46" s="10"/>
     </row>
     <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3785,7 +3842,7 @@
       <c r="D47" s="14"/>
       <c r="E47" s="15"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="36"/>
+      <c r="G47" s="35"/>
       <c r="H47" s="9"/>
       <c r="I47" s="5"/>
       <c r="J47" s="16"/>
@@ -3798,7 +3855,7 @@
       <c r="Q47" s="10"/>
       <c r="R47" s="11"/>
       <c r="S47" s="10"/>
-      <c r="T47" s="37"/>
+      <c r="T47" s="36"/>
       <c r="U47" s="10"/>
     </row>
     <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3808,7 +3865,7 @@
       <c r="D48" s="14"/>
       <c r="E48" s="15"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="36"/>
+      <c r="G48" s="35"/>
       <c r="H48" s="9"/>
       <c r="I48" s="5"/>
       <c r="J48" s="16"/>
@@ -3821,7 +3878,7 @@
       <c r="Q48" s="10"/>
       <c r="R48" s="11"/>
       <c r="S48" s="10"/>
-      <c r="T48" s="37"/>
+      <c r="T48" s="36"/>
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3831,7 +3888,7 @@
       <c r="D49" s="14"/>
       <c r="E49" s="15"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="36"/>
+      <c r="G49" s="35"/>
       <c r="H49" s="9"/>
       <c r="I49" s="5"/>
       <c r="J49" s="16"/>
@@ -3844,7 +3901,7 @@
       <c r="Q49" s="10"/>
       <c r="R49" s="11"/>
       <c r="S49" s="10"/>
-      <c r="T49" s="37"/>
+      <c r="T49" s="36"/>
       <c r="U49" s="10"/>
     </row>
     <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3854,7 +3911,7 @@
       <c r="D50" s="14"/>
       <c r="E50" s="15"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="36"/>
+      <c r="G50" s="35"/>
       <c r="H50" s="9"/>
       <c r="I50" s="5"/>
       <c r="J50" s="16"/>
@@ -3867,7 +3924,7 @@
       <c r="Q50" s="10"/>
       <c r="R50" s="11"/>
       <c r="S50" s="10"/>
-      <c r="T50" s="37"/>
+      <c r="T50" s="36"/>
       <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3877,7 +3934,7 @@
       <c r="D51" s="14"/>
       <c r="E51" s="15"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="36"/>
+      <c r="G51" s="35"/>
       <c r="H51" s="9"/>
       <c r="I51" s="5"/>
       <c r="J51" s="16"/>
@@ -3890,7 +3947,7 @@
       <c r="Q51" s="10"/>
       <c r="R51" s="11"/>
       <c r="S51" s="10"/>
-      <c r="T51" s="37"/>
+      <c r="T51" s="36"/>
       <c r="U51" s="10"/>
     </row>
     <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3900,7 +3957,7 @@
       <c r="D52" s="14"/>
       <c r="E52" s="15"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="36"/>
+      <c r="G52" s="35"/>
       <c r="H52" s="9"/>
       <c r="I52" s="5"/>
       <c r="J52" s="16"/>
@@ -3913,7 +3970,7 @@
       <c r="Q52" s="10"/>
       <c r="R52" s="11"/>
       <c r="S52" s="10"/>
-      <c r="T52" s="37"/>
+      <c r="T52" s="36"/>
       <c r="U52" s="10"/>
     </row>
     <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3923,7 +3980,7 @@
       <c r="D53" s="14"/>
       <c r="E53" s="15"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="36"/>
+      <c r="G53" s="35"/>
       <c r="H53" s="9"/>
       <c r="I53" s="5"/>
       <c r="J53" s="16"/>
@@ -3936,7 +3993,7 @@
       <c r="Q53" s="10"/>
       <c r="R53" s="11"/>
       <c r="S53" s="10"/>
-      <c r="T53" s="37"/>
+      <c r="T53" s="36"/>
       <c r="U53" s="10"/>
     </row>
     <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3946,7 +4003,7 @@
       <c r="D54" s="14"/>
       <c r="E54" s="15"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="36"/>
+      <c r="G54" s="35"/>
       <c r="H54" s="9"/>
       <c r="I54" s="5"/>
       <c r="J54" s="16"/>
@@ -3959,7 +4016,7 @@
       <c r="Q54" s="10"/>
       <c r="R54" s="11"/>
       <c r="S54" s="10"/>
-      <c r="T54" s="37"/>
+      <c r="T54" s="36"/>
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3969,7 +4026,7 @@
       <c r="D55" s="14"/>
       <c r="E55" s="15"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="36"/>
+      <c r="G55" s="35"/>
       <c r="H55" s="9"/>
       <c r="I55" s="5"/>
       <c r="J55" s="16"/>
@@ -3982,7 +4039,7 @@
       <c r="Q55" s="10"/>
       <c r="R55" s="11"/>
       <c r="S55" s="10"/>
-      <c r="T55" s="37"/>
+      <c r="T55" s="36"/>
       <c r="U55" s="10"/>
     </row>
     <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3992,7 +4049,7 @@
       <c r="D56" s="14"/>
       <c r="E56" s="15"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="36"/>
+      <c r="G56" s="35"/>
       <c r="H56" s="9"/>
       <c r="I56" s="5"/>
       <c r="J56" s="16"/>
@@ -4005,7 +4062,7 @@
       <c r="Q56" s="10"/>
       <c r="R56" s="11"/>
       <c r="S56" s="10"/>
-      <c r="T56" s="37"/>
+      <c r="T56" s="36"/>
       <c r="U56" s="10"/>
     </row>
     <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4015,7 +4072,7 @@
       <c r="D57" s="14"/>
       <c r="E57" s="15"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="36"/>
+      <c r="G57" s="35"/>
       <c r="H57" s="9"/>
       <c r="I57" s="5"/>
       <c r="J57" s="16"/>
@@ -4028,7 +4085,7 @@
       <c r="Q57" s="10"/>
       <c r="R57" s="11"/>
       <c r="S57" s="10"/>
-      <c r="T57" s="37"/>
+      <c r="T57" s="36"/>
       <c r="U57" s="10"/>
     </row>
     <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4038,7 +4095,7 @@
       <c r="D58" s="14"/>
       <c r="E58" s="15"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="36"/>
+      <c r="G58" s="35"/>
       <c r="H58" s="9"/>
       <c r="I58" s="5"/>
       <c r="J58" s="16"/>
@@ -4051,7 +4108,7 @@
       <c r="Q58" s="10"/>
       <c r="R58" s="11"/>
       <c r="S58" s="10"/>
-      <c r="T58" s="37"/>
+      <c r="T58" s="36"/>
       <c r="U58" s="10"/>
     </row>
     <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4061,7 +4118,7 @@
       <c r="D59" s="14"/>
       <c r="E59" s="15"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="36"/>
+      <c r="G59" s="35"/>
       <c r="H59" s="9"/>
       <c r="I59" s="5"/>
       <c r="J59" s="16"/>
@@ -4074,7 +4131,7 @@
       <c r="Q59" s="10"/>
       <c r="R59" s="11"/>
       <c r="S59" s="10"/>
-      <c r="T59" s="37"/>
+      <c r="T59" s="36"/>
       <c r="U59" s="10"/>
     </row>
     <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4084,7 +4141,7 @@
       <c r="D60" s="14"/>
       <c r="E60" s="15"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="36"/>
+      <c r="G60" s="35"/>
       <c r="H60" s="9"/>
       <c r="I60" s="5"/>
       <c r="J60" s="16"/>
@@ -4097,7 +4154,7 @@
       <c r="Q60" s="10"/>
       <c r="R60" s="11"/>
       <c r="S60" s="10"/>
-      <c r="T60" s="37"/>
+      <c r="T60" s="36"/>
       <c r="U60" s="10"/>
     </row>
     <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4107,7 +4164,7 @@
       <c r="D61" s="14"/>
       <c r="E61" s="15"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="36"/>
+      <c r="G61" s="35"/>
       <c r="H61" s="9"/>
       <c r="I61" s="5"/>
       <c r="J61" s="16"/>
@@ -4120,7 +4177,7 @@
       <c r="Q61" s="10"/>
       <c r="R61" s="11"/>
       <c r="S61" s="10"/>
-      <c r="T61" s="37"/>
+      <c r="T61" s="36"/>
       <c r="U61" s="10"/>
     </row>
     <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4130,7 +4187,7 @@
       <c r="D62" s="14"/>
       <c r="E62" s="15"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="36"/>
+      <c r="G62" s="35"/>
       <c r="H62" s="9"/>
       <c r="I62" s="5"/>
       <c r="J62" s="16"/>
@@ -4143,7 +4200,7 @@
       <c r="Q62" s="10"/>
       <c r="R62" s="11"/>
       <c r="S62" s="10"/>
-      <c r="T62" s="37"/>
+      <c r="T62" s="36"/>
       <c r="U62" s="10"/>
     </row>
     <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4153,7 +4210,7 @@
       <c r="D63" s="14"/>
       <c r="E63" s="15"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="36"/>
+      <c r="G63" s="35"/>
       <c r="H63" s="9"/>
       <c r="I63" s="5"/>
       <c r="J63" s="16"/>
@@ -4166,7 +4223,7 @@
       <c r="Q63" s="10"/>
       <c r="R63" s="11"/>
       <c r="S63" s="10"/>
-      <c r="T63" s="37"/>
+      <c r="T63" s="36"/>
       <c r="U63" s="10"/>
     </row>
     <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4176,7 +4233,7 @@
       <c r="D64" s="14"/>
       <c r="E64" s="15"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="36"/>
+      <c r="G64" s="35"/>
       <c r="H64" s="9"/>
       <c r="I64" s="5"/>
       <c r="J64" s="16"/>
@@ -4189,7 +4246,7 @@
       <c r="Q64" s="10"/>
       <c r="R64" s="11"/>
       <c r="S64" s="10"/>
-      <c r="T64" s="37"/>
+      <c r="T64" s="36"/>
       <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4199,7 +4256,7 @@
       <c r="D65" s="14"/>
       <c r="E65" s="15"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="36"/>
+      <c r="G65" s="35"/>
       <c r="H65" s="9"/>
       <c r="I65" s="5"/>
       <c r="J65" s="16"/>
@@ -4212,7 +4269,7 @@
       <c r="Q65" s="10"/>
       <c r="R65" s="11"/>
       <c r="S65" s="10"/>
-      <c r="T65" s="37"/>
+      <c r="T65" s="36"/>
       <c r="U65" s="10"/>
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4222,7 +4279,7 @@
       <c r="D66" s="14"/>
       <c r="E66" s="15"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="36"/>
+      <c r="G66" s="35"/>
       <c r="H66" s="9"/>
       <c r="I66" s="5"/>
       <c r="J66" s="16"/>
@@ -4235,7 +4292,7 @@
       <c r="Q66" s="10"/>
       <c r="R66" s="11"/>
       <c r="S66" s="10"/>
-      <c r="T66" s="37"/>
+      <c r="T66" s="36"/>
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4245,7 +4302,7 @@
       <c r="D67" s="14"/>
       <c r="E67" s="15"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="36"/>
+      <c r="G67" s="35"/>
       <c r="H67" s="9"/>
       <c r="I67" s="5"/>
       <c r="J67" s="16"/>
@@ -4258,7 +4315,7 @@
       <c r="Q67" s="10"/>
       <c r="R67" s="11"/>
       <c r="S67" s="10"/>
-      <c r="T67" s="37"/>
+      <c r="T67" s="36"/>
       <c r="U67" s="10"/>
     </row>
     <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4268,7 +4325,7 @@
       <c r="D68" s="14"/>
       <c r="E68" s="15"/>
       <c r="F68" s="9"/>
-      <c r="G68" s="36"/>
+      <c r="G68" s="35"/>
       <c r="H68" s="9"/>
       <c r="I68" s="5"/>
       <c r="J68" s="16"/>
@@ -4281,7 +4338,7 @@
       <c r="Q68" s="10"/>
       <c r="R68" s="11"/>
       <c r="S68" s="10"/>
-      <c r="T68" s="37"/>
+      <c r="T68" s="36"/>
       <c r="U68" s="10"/>
     </row>
     <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4291,7 +4348,7 @@
       <c r="D69" s="14"/>
       <c r="E69" s="15"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="36"/>
+      <c r="G69" s="35"/>
       <c r="H69" s="9"/>
       <c r="I69" s="5"/>
       <c r="J69" s="16"/>
@@ -4304,7 +4361,7 @@
       <c r="Q69" s="10"/>
       <c r="R69" s="11"/>
       <c r="S69" s="10"/>
-      <c r="T69" s="37"/>
+      <c r="T69" s="36"/>
       <c r="U69" s="10"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
@@ -4518,6 +4575,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -4525,31 +4583,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N69</xm:sqref>
+          <xm:sqref>N3:N18 N19:N69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A69</xm:sqref>
+          <xm:sqref>A3:A18 A19:A69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I69 P3:P69 K3:K69</xm:sqref>
+          <xm:sqref>I3:I18 I19:I69 P3:P18 P19:P69 K3:K18 K19:K69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L69</xm:sqref>
+          <xm:sqref>L3:L18 L19:L69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M69</xm:sqref>
+          <xm:sqref>M3:M18 M19:M69</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4576,16 +4634,16 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>241</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4596,7 +4654,7 @@
         <v>133</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D3" s="22"/>
     </row>
@@ -4618,7 +4676,7 @@
         <v>147</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D5" s="22"/>
     </row>
@@ -4634,29 +4692,29 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>169</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>170</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>165</v>
@@ -4666,71 +4724,71 @@
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="21" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="21" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D14" s="22"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>165</v>
@@ -4740,45 +4798,45 @@
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>165</v>
@@ -4788,7 +4846,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="16"/>
@@ -4796,7 +4854,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>10</v>
@@ -4806,41 +4864,41 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>235</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="24" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D24" s="25"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D25" s="25"/>
     </row>

</xml_diff>

<commit_message>
revisión escaletas para notificación
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/Escaleta CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/Escaleta CN_06_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="271">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1219,16 +1219,34 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1268,24 +1286,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1593,11 +1593,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,94 +1626,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="56"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="59" t="s">
+      <c r="S1" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="61" t="s">
+      <c r="T1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="59" t="s">
+      <c r="U1" s="44" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="51"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="57"/>
       <c r="M2" s="37" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="60"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="45"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1771,7 +1772,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>122</v>
       </c>
@@ -1891,7 +1892,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>122</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>122</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>122</v>
       </c>
@@ -2154,7 +2155,7 @@
       <c r="T10" s="36"/>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>122</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>122</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>122</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>122</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>122</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>122</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>122</v>
       </c>
@@ -2960,7 +2961,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>122</v>
       </c>
@@ -3021,7 +3022,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>122</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>122</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>122</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>122</v>
       </c>
@@ -3314,7 +3315,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>122</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>122</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>122</v>
       </c>
@@ -3457,7 +3458,9 @@
       <c r="J33" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="K33" s="7"/>
+      <c r="K33" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="L33" s="6" t="s">
         <v>10</v>
       </c>
@@ -4553,14 +4556,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U35"/>
+  <autoFilter ref="A2:U35">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="NO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4575,6 +4578,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>